<commit_message>
Fixed a minor bug in months where there are four Sundays/Wednesdays and the first Wednesday comes before the first Sunday. The second Wednesday would have the first Wednesday's date and every Wednesday thereafter would be a week off.
</commit_message>
<xml_diff>
--- a/output-files/Example Calendar.xlsx
+++ b/output-files/Example Calendar.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasfiveash/Desktop/Parking-Lot-Scheduler-master/output-files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomasfiveash/Desktop/Parking-Lot-Scheduler/output-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19560"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="19560"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar2" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="calFile" type="6" refreshedVersion="5" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="/Users/thomasfiveash/Desktop/Parking-Lot-Scheduler-master/output-files/calFile.csv" tab="0" comma="1">
+    <textPr codePage="437" sourceFile="/Users/thomasfiveash/Desktop/Parking-Lot-Scheduler/output-files/calFile.csv" tab="0" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
   <si>
     <t>Parking Lot Duty</t>
   </si>
@@ -159,67 +159,67 @@
     <t>Justin Wood</t>
   </si>
   <si>
+    <t>Carl Ramirez</t>
+  </si>
+  <si>
+    <t>Robert Taylor</t>
+  </si>
+  <si>
+    <t>Carl Mitchell</t>
+  </si>
+  <si>
+    <t>Jeremy Evans</t>
+  </si>
+  <si>
+    <t>Jesse Gonzales</t>
+  </si>
+  <si>
+    <t>Steve Johnson</t>
+  </si>
+  <si>
+    <t>Keith Hill</t>
+  </si>
+  <si>
+    <t>George Rogers</t>
+  </si>
+  <si>
+    <t>Chris Evans</t>
+  </si>
+  <si>
+    <t>Walter Brown</t>
+  </si>
+  <si>
+    <t>Bobby Bailey</t>
+  </si>
+  <si>
+    <t>Brian Price</t>
+  </si>
+  <si>
+    <t>Martin Rodriguez</t>
+  </si>
+  <si>
+    <t>Richard Miller</t>
+  </si>
+  <si>
+    <t>William Bryant</t>
+  </si>
+  <si>
+    <t>Steven Patterson</t>
+  </si>
+  <si>
+    <t>Larry Parker</t>
+  </si>
+  <si>
+    <t>Carlos Miller: 123-456-7890</t>
+  </si>
+  <si>
+    <t>Wayne Long</t>
+  </si>
+  <si>
+    <t>Chris Clark</t>
+  </si>
+  <si>
     <t>Peter Rivera</t>
-  </si>
-  <si>
-    <t>Carl Ramirez</t>
-  </si>
-  <si>
-    <t>Robert Taylor</t>
-  </si>
-  <si>
-    <t>Carl Mitchell</t>
-  </si>
-  <si>
-    <t>Jeremy Evans</t>
-  </si>
-  <si>
-    <t>Jesse Gonzales</t>
-  </si>
-  <si>
-    <t>Steve Johnson</t>
-  </si>
-  <si>
-    <t>Keith Hill</t>
-  </si>
-  <si>
-    <t>George Rogers</t>
-  </si>
-  <si>
-    <t>Chris Evans</t>
-  </si>
-  <si>
-    <t>Walter Brown</t>
-  </si>
-  <si>
-    <t>Bobby Bailey</t>
-  </si>
-  <si>
-    <t>Brian Price</t>
-  </si>
-  <si>
-    <t>Martin Rodriguez</t>
-  </si>
-  <si>
-    <t>Richard Miller</t>
-  </si>
-  <si>
-    <t>William Bryant</t>
-  </si>
-  <si>
-    <t>Steven Patterson</t>
-  </si>
-  <si>
-    <t>Larry Parker</t>
-  </si>
-  <si>
-    <t>Carlos Miller: 123-456-7890</t>
-  </si>
-  <si>
-    <t>Wayne Long</t>
-  </si>
-  <si>
-    <t>Chris Clark</t>
   </si>
 </sst>
 </file>
@@ -715,7 +715,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -726,7 +726,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="37" x14ac:dyDescent="0.45">
       <c r="A1" s="16">
-        <v>42370</v>
+        <v>42401</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -766,17 +766,11 @@
       <c r="E3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="14">
-        <v>42007</v>
-      </c>
-      <c r="B4" s="14">
-        <v>42007</v>
-      </c>
-      <c r="C4" s="14">
-        <v>42007</v>
-      </c>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
       <c r="D4" s="14">
-        <v>42010</v>
+        <v>42403</v>
       </c>
       <c r="E4"/>
     </row>
@@ -788,51 +782,33 @@
       <c r="E5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>42</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:5" ht="7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -841,16 +817,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="14">
-        <v>42014</v>
+        <v>42407</v>
       </c>
       <c r="B10" s="14">
-        <v>42014</v>
+        <v>42407</v>
       </c>
       <c r="C10" s="14">
-        <v>42014</v>
+        <v>42407</v>
       </c>
       <c r="D10" s="14">
-        <v>42017</v>
+        <v>42410</v>
       </c>
       <c r="E10"/>
     </row>
@@ -863,50 +839,50 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="E12"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="E13"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E14"/>
     </row>
-    <row r="15" spans="1:5" ht="7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -915,20 +891,20 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="14">
-        <v>42021</v>
+        <v>42414</v>
       </c>
       <c r="B16" s="14">
-        <v>42021</v>
+        <v>42414</v>
       </c>
       <c r="C16" s="14">
-        <v>42021</v>
+        <v>42414</v>
       </c>
       <c r="D16" s="14">
-        <v>42024</v>
+        <v>42417</v>
       </c>
       <c r="E16"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -937,50 +913,50 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="E18"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E19"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="E20"/>
     </row>
-    <row r="21" spans="1:5" ht="7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -989,16 +965,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="14">
-        <v>42028</v>
+        <v>42421</v>
       </c>
       <c r="B22" s="14">
-        <v>42028</v>
+        <v>42421</v>
       </c>
       <c r="C22" s="14">
-        <v>42028</v>
+        <v>42421</v>
       </c>
       <c r="D22" s="14">
-        <v>42031</v>
+        <v>42424</v>
       </c>
       <c r="E22"/>
     </row>
@@ -1011,50 +987,50 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="E24"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E25"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="E26"/>
     </row>
-    <row r="27" spans="1:5" ht="7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1063,13 +1039,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="14">
-        <v>42035</v>
+        <v>42428</v>
       </c>
       <c r="B28" s="14">
-        <v>42035</v>
+        <v>42428</v>
       </c>
       <c r="C28" s="14">
-        <v>42035</v>
+        <v>42428</v>
       </c>
       <c r="D28" s="14"/>
       <c r="E28"/>
@@ -1083,44 +1059,44 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32"/>
     </row>
-    <row r="33" spans="1:5" ht="7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1166,7 +1142,7 @@
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="12"/>
       <c r="B38" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C38" s="15"/>
       <c r="D38" s="12"/>

</xml_diff>